<commit_message>
implementamos interfaz grafica y conectamos con la funcionalidad del codigo
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
   <si>
     <t>Alumno</t>
   </si>
@@ -29,10 +29,19 @@
     <t>Juan</t>
   </si>
   <si>
+    <t>Amigo Personal</t>
+  </si>
+  <si>
     <t>Pedro</t>
   </si>
   <si>
+    <t>Compañero</t>
+  </si>
+  <si>
     <t>Lucas</t>
+  </si>
+  <si>
+    <t>Conocido</t>
   </si>
   <si>
     <t>Lautaro</t>
@@ -42,6 +51,9 @@
   </si>
   <si>
     <t>Jose</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
   </si>
   <si>
     <t>Agustin</t>
@@ -85,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -94,10 +106,16 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -341,80 +359,80 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
-        <v>3.0</v>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
-        <v>1.0</v>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2">
-        <v>2.0</v>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3.0</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
-        <v>1.0</v>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2.0</v>
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1.0</v>
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1438,50 +1456,50 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="4">
-        <v>3.0</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.0</v>
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1.0</v>
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4">
-        <v>3.0</v>
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D5" s="1"/>
     </row>

</xml_diff>